<commit_message>
Started cleaning the example 4-bill-test and directions in rmd
</commit_message>
<xml_diff>
--- a/4-bill-test.xlsx
+++ b/4-bill-test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdeaton\Documents\GitHub\anti-trans-legislation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4815ED77-23B9-41DF-8594-1A4216FEA3FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF7C10F0-E325-4A4F-8EC0-764D4E2A742F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17790" windowHeight="4500" xr2:uid="{32BA1DAC-DB74-DB41-A18F-C0D577D22603}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -742,6 +742,212 @@
 231 commenced within 5 years after the date of the person's death or
 232 the discovery of the person's death, whichever is later.
 233 Section 9. This act shall take effect July 1, 2023.</t>
+  </si>
+  <si>
+    <t>AN EMPLOYEE OR INDEPENDENT CONTRACTOR OF A SCHOOL DISTRICT OR CHARTER SCHOOL MAY NOT KNOWINGLY ADDRESS, IDENTIFY OR REFER TO A STUDENT WHO IS UNDER EIGHTEEN YEARS OF AGE BY EITHER OF THE FOLLOWING UNLESS THE SCHOOL DISTRICT OR CHARTER SCHOOL RECEIVES WRITTEN PERMISSION FROM THE STUDENT'S PARENT:
+A PRONOUN THAT DIFFERS FROM THE PRONOUN THAT ALIGNS WITH THE STUDENT'S BIOLOGICAL SEX.
+A FIRST NAME OTHER THAN THE FIRST OR MIDDLE NAME THAT IS LISTED ON THE STUDENT'S OFFICIAL SCHOOL RECORDS, EXCEPT THAT AN EMPLOYEE OR INDEPENDENT CONTRACTOR MAY ADDRESS, IDENTIFY OR REFER TO A STUDENT BY A NICKNAME THAT IS COMMONLY ASSOCIATED WITH THE STUDENT'S NAME OF RECORD.
+A SCHOOL DISTRICT OR CHARTER SCHOOL MAY NOT REQUIRE AN EMPLOYEE OR INDEPENDENT CONTRACTOR TO ADDRESS, IDENTIFY OR REFER TO A PERSON BY A PRONOUN THAT DIFFERS FROM THE PRONOUN THAT ALIGNS WITH THE PERSON'S BIOLOGICAL SEX IF DOING SO IS CONTRARY I3TO THE EMPLOYEE'S OR INDEPENDENT CONTRACTOR'S RELIGIOUS OR MORAL CONVICTIONS.
+EACH SCHOOL DISTRICT GOVERNING BOARD AND CHARTER SCHOOL GOVERNING BODY SHALL ADOPT POLICIES TO IMPLEMENT THIS SECTION.
+THIS SECTION DOES NOT PROHIBIT ANY PERSON DESCRIBED IN SUBSECTION A OF THIS SECTION FROM DISCUSSING MATTERS OF PUBLIC CONCERN OUTSIDE THE CONTEXT OF THE PERSON'S OFFICIAL DUTIES.</t>
+  </si>
+  <si>
+    <t>Given Name Act — Protection against compelled speech.
+This section shall be known and may be cited as the "Given Name Act"
+The General Assembly finds that:
+Faculty members, teachers, and employees of public schools and state-supported institutions of higher education do not shed their constitutional rights to freedom of speech or expression at work;
+Protecting the right to free speech for faculty members, teachers, and employees promotes three (3) important interests, which include:
+Students' interests in receiving informed opinions on matters of public concern;
+Faculty members', teachers', and employees' rights to disseminate their own opinions; and
+The public's interest in exposing our children and future leaders to different viewpoints; and
+The selection and use of pronouns in classrooms, on campuses, and elsewhere is a matter of free speech and academic freedom because it communicates a message on a matter of public concern and shapes classroom discussions and debates, and is not merely an administrative or ministerial act by faculty members, teachers, and employees of public schools and state-supported institutions of higher education.
+As used in this section, "school" includes:
+A public school or school district;
+An open-enrollment public charter school; and
+A state-supported institution of higher education.
+A faculty member, teacher, or other employee of a school, regardless of the scope of his or her official duties:
+Shall not address an unemancipated minor or student with a:
+Pronoun or title that is inconsistent with the unemancipated minor's or student's biological sex unless the faculty member, teacher, or other employee of a school has the written permission of the unemancipated minor's or student's parent, legal guardian, or person standing in loco parentis to the unemancipated minor or student if the unemancipated minor or student is under eighteen (18) years of age; or Name other than the name listed on the unemancipated minor's or student's birth certificate, or a derivative of the name listed on the unemancipated minor's or student's birth certificate, without the written permission of the unemancipated minor's or student's parent, legal guardian, or person standing in loco parentis to the unemancipated minor or student if the unemancipated minor or student is under eighteen (18) years of age; and
+Notwithstanding subdivision (d)(1) of this section, shall not be subject to adverse employment action for declining to address a person using a:
+Name other than the name listed on the person's birth certificate; or
+Pronoun or title that is inconsistent with the person's biological sex.
+A student shall not be subject to any disciplinary action for declining to address a person using a:
+Name other than the name listed on the person's birth certificate; or
+Pronoun or title that is inconsistent with the person's biological sex.
+A person who is harmed by a violation of this section may bring a cause of action for:
+Injunctive relief;
+Monetary damages;
+Reasonable attorney's fees and costs; and
+Any other appropriate relief.</t>
+  </si>
+  <si>
+    <t>Temporary emergency jurisdiction.—
+A court of this state has temporary emergency jurisdiction if the child is present in this state and:
+The child has been abandoned; or
+It is necessary in an emergency to protect the child because the child, or a sibling or parent of the child, is subjected to or threatened with mistreatment or abuse; or
+It is necessary in an emergency to protect the child because the child has been subjected to or is threatened with being subjected to sex-reassignment prescriptions or procedures, as defined in s. 456.001.
+Warrant to take physical custody of child.—
+Upon the filing of a petition seeking enforcement of a child custody determination, the petitioner may file a verified application for the issuance of a warrant to take physical custody of the child if the child is likely to imminently suffer serious physical harm or removal from this state. Serious physical harm includes, but is not limited to, being subjected to sex-reassignment prescriptions or procedures as defined in s. 456.001.
+Prohibited use of state funds.—
+As used in this section, the term “governmental entity” means the state or any political subdivision thereof, including the executive, legislative, and judicial branches of government; the independent establishments of the state, counties, municipalities, districts, authorities, boards, or commissions; and any agencies that are subject to chapter 286.
+A governmental entity, a public postsecondary educational institution as described in s. 1000.04, the state group health insurance program, a managing entity as defined in s. 394.9082, or a managed care plan providing services under part IV of chapter 409 may not expend state funds as described in s. 215.31 for sex-reassignment prescriptions or procedures as defined in s. 456.001.
+Definitions.—As used in this chapter, the term:
+“Sex” means the classification of a person as either male or female based on the organization of the human body of such person for a specific reproductive role, as indicated by the person’s sex chromosomes, naturally occurring sex hormones, and internal and external genitalia present at birth.
+“Sex-reassignment prescriptions or procedures” means:
+The prescription or administration of puberty blockers for the purpose of attempting to stop or delay normal puberty in order to affirm a person’s perception of his or her sex if that perception is inconsistent with the person’s sex as defined in subsection (8).
+The prescription or administration of hormones or hormone antagonists to affirm a person’s perception of his or her sex if that perception is inconsistent with the person’s sex as defined in subsection (8).
+Any medical procedure, including a surgical procedure, to affirm a person’s perception of his or her sex if that
+  120  perception is inconsistent with the person’s sex as defined in subsection (8).
+  122         (b) The term does not include:
+  123         1. Treatment provided by a physician who, in his or her
+  124  good faith clinical judgment, performs procedures upon or
+  125  provides therapies to a minor born with a medically verifiable
+  126  genetic disorder of sexual development, including any of the
+  127  following:
+  128         a. External biological sex characteristics that are
+  129  unresolvably ambiguous.
+  130         b. A disorder of sexual development in which the physician
+  131  has determined through genetic or biochemical testing that the
+  132  patient does not have a normal sex chromosome structure, sex
+  133  steroid hormone production, or sex steroid hormone action for a
+  134  male or female, as applicable.
+  135         2. Prescriptions or procedures to treat an infection, an
+  136  injury, a disease, or a disorder that has been caused or
+  137  exacerbated by the performance of any sex-reassignment
+  138  prescription or procedure, regardless of whether such
+  139  prescription or procedure was performed in accordance with state
+  140  or federal law.
+  141         3. Prescriptions or procedures provided to a patient for
+  142  the treatment of a physical disorder, physical injury, or
+  143  physical illness that would, as certified by a physician
+  144  licensed under chapter 458 or chapter 459, place the individual
+  145  in imminent danger of death or impairment of a major bodily
+  146  function without the prescription or procedure.
+  147         Section 5. Section 456.52, Florida Statutes, is created to
+  148  read:
+  149         456.52 Sex-reassignment prescriptions and procedures;
+  150  prohibitions; informed consent.—
+  151         (1) Sex-reassignment prescriptions and procedures are
+  152  prohibited for patients younger than 18 years of age, except
+  153  that:
+  154         (a) The Board of Medicine and the Board of Osteopathic
+  155  Medicine shall, within 60 days after the effective date of this
+  156  act, adopt emergency rules pertaining to standards of practice
+  157  under which a patient younger than 18 years of age may continue
+  158  to be treated with a prescription consistent with those
+  159  referenced under s. 456.001(9)(a)1. or 2. if such treatment for
+  160  sex reassignment was commenced before, and is still active on,
+  161  the effective date of this act. In developing rules under this
+  162  paragraph, the boards shall consider requirements for physicians
+  163  to obtain informed consent from such patient′s parent or legal
+  164  guardian, consistent with the parameters of informed consent
+  165  under subsections (2) and (4), for such prescription treatment,
+  166  and shall consider the provision of professional counseling
+  167  services for such patient by a board-certified psychiatrist
+  168  licensed under chapter 458 or chapter 459 or a psychologist
+  169  licensed under chapter 490 in conjunction with such prescription
+  170  treatment.
+  171         (b) A patient meeting the criteria of paragraph (a) may
+  172  continue to be treated by a physician with such prescriptions
+  173  according to rules adopted under paragraph (a) or nonemergency
+  174  rules adopted under paragraph (6)(b).
+  175         (2) If sex-reassignment prescriptions or procedures are
+  176  prescribed for or administered or performed on patients 18 years
+  177  of age or older, consent must be voluntary, informed, and in
+  178  writing on forms adopted in rule by the Board of Medicine and
+  179  the Board of Osteopathic Medicine. Consent to sex-reassignment
+  180  prescriptions or procedures is voluntary and informed only if
+  181  the physician who is to prescribe or administer the
+  182  pharmaceutical product or perform the procedure has, at a
+  183  minimum, while physically present in the same room:
+  184         (a) Informed the patient of the nature and risks of the
+  185  prescription or procedure in order for the patient to make a
+  186  prudent decision;
+  187         (b) Provided the informed consent form, as adopted in rule
+  188  by the Board of Medicine and the Board of Osteopathic Medicine,
+  189  to the patient; and
+  190         (c) Received the patient’s written acknowledgment, before
+  191  the prescription or procedure is prescribed, administered, or
+  192  performed, that the information required to be provided under
+  193  this subsection has been provided.
+  194         (3) Sex-reassignment prescriptions or procedures may not be
+  195  prescribed, administered, or performed except by a physician.
+  196  For the purposes of this section, the term “physician” is
+  197  defined as a physician licensed under chapter 458 or chapter 459
+  198  or a physician practicing medicine or osteopathic medicine in
+  199  the employment of the Federal Government.
+  200         (4) Consent required under subsection (2) does not apply to
+  201  renewals of prescriptions consistent with those referenced under
+  202  s. 456.001(9)(a)1. and 2. if a physician and his or her patient
+  203  have met the requirements for consent for the initial
+  204  prescription or renewal. However, separate consent is required
+  205  for any new prescription for a pharmaceutical product not
+  206  previously prescribed to the patient.
+  207         (5)(a) Violation of this section constitutes grounds for
+  208  disciplinary action under this chapter and chapter 458 or
+  209  chapter 459, as applicable.
+  210         (b) Any health care practitioner who willfully or actively
+  211  participates in a violation of subsection (1) commits a felony
+  212  of the third degree, punishable as provided in s. 775.082, s.
+  213  775.083, or s. 775.084.
+  214         (c) Any health care practitioner who violates subsection
+  215  (2), subsection (3), or subsection (4) commits a misdemeanor of
+  216  the first degree, punishable as provided in s. 775.082 or s.
+  217  775.083.
+  218         (6)(a) The Board of Medicine and the Board of Osteopathic
+  219  Medicine shall adopt emergency rules to implement this section.
+  220         (b) Any emergency rules adopted under this section are
+  221  exempt from s. 120.54(4)(c) and shall remain in effect until
+  222  replaced by rules adopted under the nonemergency rulemaking
+  223  procedures of the Administrative Procedure Act.
+  224         Section 6. Present paragraphs (c) through (gg) of
+  225  subsection (5) of section 456.074, Florida Statutes, are
+  226  redesignated as paragraphs (d) through (hh), respectively, and a
+  227  new paragraph (c) is added to that subsection, to read:
+  228         456.074 Certain health care practitioners; immediate
+  229  suspension of license.—
+  230         (5) The department shall issue an emergency order
+  231  suspending the license of any health care practitioner who is
+  232  arrested for committing or attempting, soliciting, or conspiring
+  233  to commit any act that would constitute a violation of any of
+  234  the following criminal offenses in this state or similar
+  235  offenses in another jurisdiction:
+  236         (c) Section 456.52(5)(b), relating to prescribing,
+  237  administering, or performing sex-reassignment prescriptions or
+  238  procedures for a patient younger than 18 years of age.
+  239         Section 7. Section 766.318, Florida Statutes, is created to
+  240  read:
+  241         766.318 Civil liability for provision of sex-reassignment
+  242  prescriptions or procedures to minors.—
+  243         (1) A cause of action exists to recover damages for
+  244  personal injury or death resulting from the provision of sex
+  245  reassignment prescriptions or procedures, as defined in s.
+  246  456.001, to a person younger than 18 years of age which are
+  247  prohibited by s. 456.52(1).
+  248         (2) The limitations on punitive damages in s. 768.73(1) do
+  249  not apply to actions brought under this section.
+  250         (3) An action brought under this section:
+  251         (a) May be commenced within 20 years after the cessation or
+  252  completion of the sex-reassignment prescription or procedure.
+  253         (b) Is in addition to any other remedy authorized by law.
+  254         (4) The cause of action created by this section does not
+  255  apply to:
+  256         (a) Treatment with sex-reassignment prescriptions if such
+  257  treatment is consistent with s. 456.001(9)(a)1. or 2. and was
+  258  commenced on or before, and is still active on, the effective
+  259  date of this act.
+  260         (b) Sex-reassignment prescriptions or procedures that were
+  261  ceased or completed on or before the effective date of this act.
+  262         Section 8. If any provision of this act or its application
+  263  to any person or circumstance is held invalid, the invalidity
+  264  does not affect other provisions or applications of this act
+  265  which can be given effect without the invalid provision or
+  266  application, and to this end the provisions of this act are
+  267  severable.
+  268         Section 9. The Division of Law Revision is directed to
+  269  replace the phrase “the effective date of this act” wherever it
+  270  occurs in this act with the date this act becomes a law.
+  271         Section 10. This act shall take effect upon becoming a law.</t>
   </si>
 </sst>
 </file>
@@ -1108,10 +1314,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{968883DB-AF00-B64D-9E18-9ACE2911B86F}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1119,9 +1325,10 @@
     <col min="4" max="4" width="29.83203125" customWidth="1"/>
     <col min="7" max="7" width="31.5" customWidth="1"/>
     <col min="8" max="8" width="69.5" customWidth="1"/>
+    <col min="9" max="9" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1147,7 +1354,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>45065</v>
       </c>
@@ -1172,8 +1379,11 @@
       <c r="H2" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="I2" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" ht="409" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="409" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>45027</v>
       </c>
@@ -1198,8 +1408,11 @@
       <c r="H3" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="I3" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>45064</v>
       </c>
@@ -1224,8 +1437,11 @@
       <c r="H4" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="I4" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>44988</v>
       </c>
@@ -1250,11 +1466,14 @@
       <c r="H5" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="I5" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more data cleaning stuff
</commit_message>
<xml_diff>
--- a/4-bill-test.xlsx
+++ b/4-bill-test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdeaton\Documents\GitHub\anti-trans-legislation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF7C10F0-E325-4A4F-8EC0-764D4E2A742F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A6A580-0B17-4CBE-86E8-2690DC79C97C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17790" windowHeight="4500" xr2:uid="{32BA1DAC-DB74-DB41-A18F-C0D577D22603}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -796,158 +796,96 @@
 “Sex-reassignment prescriptions or procedures” means:
 The prescription or administration of puberty blockers for the purpose of attempting to stop or delay normal puberty in order to affirm a person’s perception of his or her sex if that perception is inconsistent with the person’s sex as defined in subsection (8).
 The prescription or administration of hormones or hormone antagonists to affirm a person’s perception of his or her sex if that perception is inconsistent with the person’s sex as defined in subsection (8).
-Any medical procedure, including a surgical procedure, to affirm a person’s perception of his or her sex if that
-  120  perception is inconsistent with the person’s sex as defined in subsection (8).
-  122         (b) The term does not include:
-  123         1. Treatment provided by a physician who, in his or her
-  124  good faith clinical judgment, performs procedures upon or
-  125  provides therapies to a minor born with a medically verifiable
-  126  genetic disorder of sexual development, including any of the
-  127  following:
-  128         a. External biological sex characteristics that are
-  129  unresolvably ambiguous.
-  130         b. A disorder of sexual development in which the physician
-  131  has determined through genetic or biochemical testing that the
-  132  patient does not have a normal sex chromosome structure, sex
-  133  steroid hormone production, or sex steroid hormone action for a
-  134  male or female, as applicable.
-  135         2. Prescriptions or procedures to treat an infection, an
-  136  injury, a disease, or a disorder that has been caused or
-  137  exacerbated by the performance of any sex-reassignment
-  138  prescription or procedure, regardless of whether such
-  139  prescription or procedure was performed in accordance with state
-  140  or federal law.
-  141         3. Prescriptions or procedures provided to a patient for
-  142  the treatment of a physical disorder, physical injury, or
-  143  physical illness that would, as certified by a physician
-  144  licensed under chapter 458 or chapter 459, place the individual
-  145  in imminent danger of death or impairment of a major bodily
-  146  function without the prescription or procedure.
-  147         Section 5. Section 456.52, Florida Statutes, is created to
-  148  read:
-  149         456.52 Sex-reassignment prescriptions and procedures;
-  150  prohibitions; informed consent.—
-  151         (1) Sex-reassignment prescriptions and procedures are
-  152  prohibited for patients younger than 18 years of age, except
-  153  that:
-  154         (a) The Board of Medicine and the Board of Osteopathic
-  155  Medicine shall, within 60 days after the effective date of this
-  156  act, adopt emergency rules pertaining to standards of practice
-  157  under which a patient younger than 18 years of age may continue
-  158  to be treated with a prescription consistent with those
-  159  referenced under s. 456.001(9)(a)1. or 2. if such treatment for
-  160  sex reassignment was commenced before, and is still active on,
-  161  the effective date of this act. In developing rules under this
-  162  paragraph, the boards shall consider requirements for physicians
-  163  to obtain informed consent from such patient′s parent or legal
-  164  guardian, consistent with the parameters of informed consent
-  165  under subsections (2) and (4), for such prescription treatment,
-  166  and shall consider the provision of professional counseling
-  167  services for such patient by a board-certified psychiatrist
-  168  licensed under chapter 458 or chapter 459 or a psychologist
-  169  licensed under chapter 490 in conjunction with such prescription
-  170  treatment.
-  171         (b) A patient meeting the criteria of paragraph (a) may
-  172  continue to be treated by a physician with such prescriptions
-  173  according to rules adopted under paragraph (a) or nonemergency
-  174  rules adopted under paragraph (6)(b).
-  175         (2) If sex-reassignment prescriptions or procedures are
-  176  prescribed for or administered or performed on patients 18 years
-  177  of age or older, consent must be voluntary, informed, and in
-  178  writing on forms adopted in rule by the Board of Medicine and
-  179  the Board of Osteopathic Medicine. Consent to sex-reassignment
-  180  prescriptions or procedures is voluntary and informed only if
-  181  the physician who is to prescribe or administer the
-  182  pharmaceutical product or perform the procedure has, at a
-  183  minimum, while physically present in the same room:
-  184         (a) Informed the patient of the nature and risks of the
-  185  prescription or procedure in order for the patient to make a
-  186  prudent decision;
-  187         (b) Provided the informed consent form, as adopted in rule
-  188  by the Board of Medicine and the Board of Osteopathic Medicine,
-  189  to the patient; and
-  190         (c) Received the patient’s written acknowledgment, before
-  191  the prescription or procedure is prescribed, administered, or
-  192  performed, that the information required to be provided under
-  193  this subsection has been provided.
-  194         (3) Sex-reassignment prescriptions or procedures may not be
-  195  prescribed, administered, or performed except by a physician.
-  196  For the purposes of this section, the term “physician” is
-  197  defined as a physician licensed under chapter 458 or chapter 459
-  198  or a physician practicing medicine or osteopathic medicine in
-  199  the employment of the Federal Government.
-  200         (4) Consent required under subsection (2) does not apply to
-  201  renewals of prescriptions consistent with those referenced under
-  202  s. 456.001(9)(a)1. and 2. if a physician and his or her patient
-  203  have met the requirements for consent for the initial
-  204  prescription or renewal. However, separate consent is required
-  205  for any new prescription for a pharmaceutical product not
-  206  previously prescribed to the patient.
-  207         (5)(a) Violation of this section constitutes grounds for
-  208  disciplinary action under this chapter and chapter 458 or
-  209  chapter 459, as applicable.
-  210         (b) Any health care practitioner who willfully or actively
-  211  participates in a violation of subsection (1) commits a felony
-  212  of the third degree, punishable as provided in s. 775.082, s.
-  213  775.083, or s. 775.084.
-  214         (c) Any health care practitioner who violates subsection
-  215  (2), subsection (3), or subsection (4) commits a misdemeanor of
-  216  the first degree, punishable as provided in s. 775.082 or s.
-  217  775.083.
-  218         (6)(a) The Board of Medicine and the Board of Osteopathic
-  219  Medicine shall adopt emergency rules to implement this section.
-  220         (b) Any emergency rules adopted under this section are
-  221  exempt from s. 120.54(4)(c) and shall remain in effect until
-  222  replaced by rules adopted under the nonemergency rulemaking
-  223  procedures of the Administrative Procedure Act.
-  224         Section 6. Present paragraphs (c) through (gg) of
-  225  subsection (5) of section 456.074, Florida Statutes, are
-  226  redesignated as paragraphs (d) through (hh), respectively, and a
-  227  new paragraph (c) is added to that subsection, to read:
-  228         456.074 Certain health care practitioners; immediate
-  229  suspension of license.—
-  230         (5) The department shall issue an emergency order
-  231  suspending the license of any health care practitioner who is
-  232  arrested for committing or attempting, soliciting, or conspiring
-  233  to commit any act that would constitute a violation of any of
-  234  the following criminal offenses in this state or similar
-  235  offenses in another jurisdiction:
-  236         (c) Section 456.52(5)(b), relating to prescribing,
-  237  administering, or performing sex-reassignment prescriptions or
-  238  procedures for a patient younger than 18 years of age.
-  239         Section 7. Section 766.318, Florida Statutes, is created to
-  240  read:
-  241         766.318 Civil liability for provision of sex-reassignment
-  242  prescriptions or procedures to minors.—
-  243         (1) A cause of action exists to recover damages for
-  244  personal injury or death resulting from the provision of sex
-  245  reassignment prescriptions or procedures, as defined in s.
-  246  456.001, to a person younger than 18 years of age which are
-  247  prohibited by s. 456.52(1).
-  248         (2) The limitations on punitive damages in s. 768.73(1) do
-  249  not apply to actions brought under this section.
-  250         (3) An action brought under this section:
-  251         (a) May be commenced within 20 years after the cessation or
-  252  completion of the sex-reassignment prescription or procedure.
-  253         (b) Is in addition to any other remedy authorized by law.
-  254         (4) The cause of action created by this section does not
-  255  apply to:
-  256         (a) Treatment with sex-reassignment prescriptions if such
-  257  treatment is consistent with s. 456.001(9)(a)1. or 2. and was
-  258  commenced on or before, and is still active on, the effective
-  259  date of this act.
-  260         (b) Sex-reassignment prescriptions or procedures that were
-  261  ceased or completed on or before the effective date of this act.
-  262         Section 8. If any provision of this act or its application
-  263  to any person or circumstance is held invalid, the invalidity
-  264  does not affect other provisions or applications of this act
-  265  which can be given effect without the invalid provision or
-  266  application, and to this end the provisions of this act are
-  267  severable.
-  268         Section 9. The Division of Law Revision is directed to
-  269  replace the phrase “the effective date of this act” wherever it
-  270  occurs in this act with the date this act becomes a law.
-  271         Section 10. This act shall take effect upon becoming a law.</t>
+Any medical procedure, including a surgical procedure, to affirm a person’s perception of his or her sex if that perception is inconsistent with the person’s sex as defined in subsection (8).
+The term does not include:
+Treatment provided by a physician who, in his or her good faith clinical judgment, performs procedures upon or provides therapies to a minor born with a medically verifiable genetic disorder of sexual development, including any of the following:
+External biological sex characteristics that are unresolvably ambiguous.
+A disorder of sexual development in which the physician has determined through genetic or biochemical testing that the patient does not have a normal sex chromosome structure, sex steroid hormone production, or sex steroid hormone action for a male or female, as applicable.
+Prescriptions or procedures to treat an infection, an injury, a disease, or a disorder that has been caused or exacerbated by the performance of any sex-reassignment prescription or procedure, regardless of whether such prescription or procedure was performed in accordance with state or federal law.
+Prescriptions or procedures provided to a patient for the treatment of a physical disorder, physical injury, or physical illness that would, as certified by a physician licensed under chapter 458 or chapter 459, place the individual in imminent danger of death or impairment of a major bodily function without the prescription or procedure.
+Sex-reassignment prescriptions and procedures; prohibitions; informed consent.—
+Sex-reassignment prescriptions and procedures are prohibited for patients younger than 18 years of age, except that:
+The Board of Medicine and the Board of Osteopathic Medicine shall, within 60 days after the effective date of this act, adopt emergency rules pertaining to standards of practice under which a patient younger than 18 years of age may continue to be treated with a prescription consistent with those referenced under s. 456.001(9)(a)1. or 2. if such treatment for sex reassignment was commenced before, and is still active on, the effective date of this act. In developing rules under this paragraph, the boards shall consider requirements for physicians to obtain informed consent from such patient′s parent or legal guardian, consistent with the parameters of informed consent under subsections (2) and (4), for such prescription treatment, and shall consider the provision of professional counseling services for such patient by a board-certified psychiatrist licensed under chapter 458 or chapter 459 or a psychologist licensed under chapter 490 in conjunction with such prescription treatment.
+A patient meeting the criteria of paragraph (a) may continue to be treated by a physician with such prescriptions according to rules adopted under paragraph (a) or nonemergency rules adopted under paragraph (6)(b).
+If sex-reassignment prescriptions or procedures are prescribed for or administered or performed on patients 18 years of age or older, consent must be voluntary, informed, and in writing on forms adopted in rule by the Board of Medicine and the Board of Osteopathic Medicine. Consent to sex-reassignment prescriptions or procedures is voluntary and informed only if the physician who is to prescribe or administer the pharmaceutical product or perform the procedure has, at a minimum, while physically present in the same room:
+Informed the patient of the nature and risks of the prescription or procedure in order for the patient to make a prudent decision;
+Provided the informed consent form, as adopted in rule by the Board of Medicine and the Board of Osteopathic Medicine, to the patient; and
+Received the patient’s written acknowledgment, before the prescription or procedure is prescribed, administered, or performed, that the information required to be provided under this subsection has been provided.
+Sex-reassignment prescriptions or procedures may not be prescribed, administered, or performed except by a physician. For the purposes of this section, the term “physician” is defined as a physician licensed under chapter 458 or chapter 459 or a physician practicing medicine or osteopathic medicine in the employment of the Federal Government.
+Consent required under subsection (2) does not apply to renewals of prescriptions consistent with those referenced under s. 456.001(9)(a)1. and 2. if a physician and his or her patient have met the requirements for consent for the initial prescription or renewal. However, separate consent is required for any new prescription for a pharmaceutical product not previously prescribed to the patient.
+Violation of this section constitutes grounds for disciplinary action under this chapter and chapter 458 or chapter 459, as applicable.
+Any health care practitioner who willfully or actively participates in a violation of subsection (1) commits a felony of the third degree, punishable as provided in s. 775.082, s. 775.083, or s. 775.084.
+Any health care practitioner who violates subsection (2), subsection (3), or subsection (4) commits a misdemeanor of the first degree, punishable as provided in s. 775.082 or s. 775.083.
+The Board of Medicine and the Board of Osteopathic Medicine shall adopt emergency rules to implement this section.
+Any emergency rules adopted under this section are exempt from s. 120.54(4)(c) and shall remain in effect until replaced by rules adopted under the nonemergency rulemaking procedures of the Administrative Procedure Act.
+Present paragraphs (c) through (gg) of subsection (5) of section 456.074, Florida Statutes, are redesignated as paragraphs (d) through (hh), respectively, and a new paragraph (c) is added to that subsection, to read:
+Certain health care practitioners; immediate suspension of license.—
+The department shall issue an emergency order suspending the license of any health care practitioner who is arrested for committing or attempting, soliciting, or conspiring to commit any act that would constitute a violation of any of the following criminal offenses in this state or similar offenses in another jurisdiction:
+Section 456.52(5)(b), relating to prescribing, administering, or performing sex-reassignment prescriptions or procedures for a patient younger than 18 years of age.
+Civil liability for provision of sex-reassignment prescriptions or procedures to minors.—
+A cause of action exists to recover damages for personal injury or death resulting from the provision of sex reassignment prescriptions or procedures, as defined in s. 456.001, to a person younger than 18 years of age which are prohibited by s. 456.52(1).
+The limitations on punitive damages in s. 768.73(1) do not apply to actions brought under this section.
+An action brought under this section:
+May be commenced within 20 years after the cessation or completion of the sex-reassignment prescription or procedure.
+Is in addition to any other remedy authorized by law.
+The cause of action created by this section does not apply to:
+Treatment with sex-reassignment prescriptions if such treatment is consistent with s. 456.001(9)(a)1. or 2. and was commenced on or before, and is still active on, the effective date of this act.
+Sex-reassignment prescriptions or procedures that were ceased or completed on or before the effective date of this act.
+If any provision of this act or its application to any person or circumstance is held invalid, the invalidity does not affect other provisions or applications of this act which can be given effect without the invalid provision or application, and to this end the provisions of this act are severable.
+The Division of Law Revision is directed to replace the phrase “the effective date of this act” wherever it occurs in this act with the date this act becomes a law.
+This act shall take effect upon becoming a law.</t>
+  </si>
+  <si>
+    <t>Protection of children from gender clinical interventions.—
+Notwithstanding any other provision of this part, a court of this state has jurisdiction to enter, modify, or stay a child custody determination relating to a child who is present in this state to the extent necessary to protect the child from being subjected to gender clinical interventions, as defined in s. 456.52(1), in another state.
+Public expenditures for gender clinical interventions; prohibition.—
+A state agency, political subdivision, public postsecondary institution as defined in 1000.04, or person providing services to or on behalf of any such agency, subdivision, or institution by contract or other agreement or relationship, may not expend funds to provide or reimburse for gender clinical interventions as defined in s. 456.52(1).
+Amendment of records.—The department, upon receipt of the fee prescribed in s. 382.0255; documentary evidence, as specified by rule, of any misstatement, error, or omission occurring in any birth, death, or fetal death record; and an affidavit setting forth the changes to be made, shall amend or replace the original certificate as necessary.
+CERTIFICATE OF LIVE BIRTH AMENDMENT.—
+The sex recorded on a birth certificate must be the person's biological sex at birth. The sex recorded on the birth certificate may only be changed in the case of a scrivener's error or in the case of a person born with external biological sex characteristics that were unresolvably ambiguous at the time of birth. The sex recorded on a birth certificate may not be changed for the purpose of affirming a person's perception of his or her sex if that perception is inconsistent with the person's sex at birth. The department may change the sex recorded on a birth certificate under this paragraph upon the written request of a health care practitioner, as defined in s. 456.001, stating and providing evidence establishing the basis for the correction. Misrepresenting or providing fraudulent evidence in such a request is grounds for disciplinary action under s. 456.072 and any applicable practice act.
+Certain health care practitioners; immediate suspension of license.—
+The department shall issue an emergency order suspending the license of any health care practitioner who is arrested for committing or attempting, soliciting, or conspiring to commit any act that would constitute a violation of any of the following criminal offenses in this state or similar offenses in another jurisdiction:
+Section 456.52(7), relating to providing gender clinical interventions to a minor.
+Prohibition on gender clinical interventions for minors; physician requirements.—
+For the purposes of this section, "gender clinical interventions" means procedures or therapies that alter internal or external physical traits for the purpose of affirming a person's perception of his or her sex if that perception is inconsistent with the person's sex at birth.
+The term includes, but is not limited to:
+Sex reassignment surgeries or any other surgical procedures that alter primary or secondary sexual characteristics.
+Puberty blocking, hormone, and hormone antagonistic therapies.
+The term does not include:
+Treatment provided by a physician who, in his or her good faith clinical judgment, performs procedures upon, or provides therapies to, a minor born with a medically verifiable genetic disorder of sexual development, including the following:
+External biological sex characteristics that are unresolvably ambiguous.
+A disorder of sexual development, in which the physician has determined through genetic or biochemical testing that the minor does not have normal sex chromosome structure, sex steroid hormone production, or sex steroid hormone action for a male or female.
+Treatment of any infection, injury, disease, or disorder caused or exacerbated by the performance of gender clinical interventions regardless of whether such interventions were performed in accordance with state or federal law.
+Gender clinical interventions may only be provided by a physician licensed under chapter 458 or chapter 459 or a physician practicing medicine or osteopathic medicine in the employment of the Federal Government.
+A physician may not provide gender clinical interventions to a minor, except that a minor who was prescribed gender clinical interventions described in (1)(a)2. on or before January 1, 2023, and continuously received such therapies through July 1, 2023, may continue to receive such therapies through December 31, 2023, solely for the purpose of gradual discontinuation of such therapies.
+Notwithstanding ss. 458.320(5) and 459.0085(5), a physician who provides gender clinical interventions for adults must obtain and maintain professional liability coverage in the amounts established in ss. 458.320(2)(b) and 459.0085(2)(b), as applicable.
+A physician must, while physically present in the same room as an adult patient, obtain informed written consent from the patient each time the physician provides gender clinical interventions. The physician must sign the consent and maintain the consent in the medical record. The patient must sign the informed consent acknowledging that the physician has sufficiently explained its content. The physician must use an informed consent form adopted in rule by the Board of Medicine and the Board of Osteopathic Medicine, which must include, at a minimum, information related to the current state of research of:
+The long-term and short-term effects of gender clinical interventions.
+The impact of gender clinical interventions on physical and mental health.
+The Board of Medicine and the Board of Osteopathic Medicine, as applicable, shall adopt emergency rules to implement this section. Any emergency rules adopted under this section are exempt from s. 120.54(4)(c) and shall remain in effect until replaced by rules adopted under the nonemergency rulemaking procedures of the Administrative Procedure Act.
+This section does not require a person to participate in a gender clinical intervention. A person is not liable for the refusal to participate in a gender clinical intervention. A person who is a member of or associated with the staff of a hospital, or an employee of a hospital or physician in which or by whom gender clinical interventions are authorized, performed, or provided, and states an objection to such intervention on clinical, moral, or religious grounds is not required to participate in such intervention. The refusal of any such person may not form the basis for any disciplinary or other recriminatory action against such person.
+A board, or the department if there is no board, must revoke the license of a health care practitioner if the board, or the department if there is no board, determines that the health care practitioner violated this section.
+A health care practitioner who willfully or actively participates in a violation of (2)(b) commits a felony of the third degree, punishable as provided in s. 775.082, s. 775.083,or s. 775.084.
+Coverage of certain treatment.—
+A health insurance policy may not provide coverage for gender clinical interventions as defined in s. 456.52(1).
+Health maintenance contracts.— 
+A health maintenance contract may not include coverage for gender clinical interventions as defined in s. 456.52(1).
+Gender clinical interventions; liability.—
+A physician who provides gender clinical interventions, as defined in s. 456.52, to a person is liable to the person for any physical, psychological, emotional, or physiological injury resulting from the gender clinical intervention.
+A person who receives a gender clinical intervention from a physician may bring a civil action against such practitioner in a court of competent jurisdiction for:
+Declaratory or injunctive relief.
+Economic damages.
+Noneconomic damages.
+Punitive damages.
+Attorney fees and costs.
+In an action brought under this section, the limitations on punitive damages in s. 768.73, or any other provision of law that seeks to limit punitive damages, do not apply.
+The estate of, or a legal guardian on behalf of, a person who received a gender clinical intervention from a physician, when the death of that person was caused by such gender clinical intervention, may bring a civil action against such practitioner in a court of competent jurisdiction for all of the following:
+All remedies available under subsection (2).
+All remedies available under s. 766.102.
+Treble damages.
+Notwithstanding s. 95.11, an action brought under subsection (2) must be commenced within 30 years after the date of the gender clinical interventions.
+An action brought under subsection (4) must be commenced within 5 years after the date of the person's death or the discovery of the person's death, whichever is later.
+This act shall take effect July 1, 2023.</t>
   </si>
 </sst>
 </file>
@@ -1316,8 +1254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{968883DB-AF00-B64D-9E18-9ACE2911B86F}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="H5" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1467,7 +1405,7 @@
         <v>31</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
finished cleaning and added template ones
</commit_message>
<xml_diff>
--- a/4-bill-test.xlsx
+++ b/4-bill-test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdeaton\Documents\GitHub\anti-trans-legislation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A6A580-0B17-4CBE-86E8-2690DC79C97C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1298DB2-2464-4C28-8167-096FB293AB35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17790" windowHeight="4500" xr2:uid="{32BA1DAC-DB74-DB41-A18F-C0D577D22603}"/>
   </bookViews>
@@ -1254,8 +1254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{968883DB-AF00-B64D-9E18-9ACE2911B86F}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H5" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
updated to multiple bills with appropriate naming reflecting the bills, added column names to xlsx files that were missing
</commit_message>
<xml_diff>
--- a/4-bill-test.xlsx
+++ b/4-bill-test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdeaton\Documents\GitHub\anti-trans-legislation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1298DB2-2464-4C28-8167-096FB293AB35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E86BCF-B125-42FE-AE6F-34BFC8F9F94D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17790" windowHeight="4500" xr2:uid="{32BA1DAC-DB74-DB41-A18F-C0D577D22603}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -886,6 +886,9 @@
 Notwithstanding s. 95.11, an action brought under subsection (2) must be commenced within 30 years after the date of the gender clinical interventions.
 An action brought under subsection (4) must be commenced within 5 years after the date of the person's death or the discovery of the person's death, whichever is later.
 This act shall take effect July 1, 2023.</t>
+  </si>
+  <si>
+    <t>text</t>
   </si>
 </sst>
 </file>
@@ -1254,8 +1257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{968883DB-AF00-B64D-9E18-9ACE2911B86F}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1290,6 +1293,9 @@
       </c>
       <c r="H1" t="s">
         <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
added a bill 5 that a judge commented on for use in the oer case study
</commit_message>
<xml_diff>
--- a/4-bill-test.xlsx
+++ b/4-bill-test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdeaton\Documents\GitHub\anti-trans-legislation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E86BCF-B125-42FE-AE6F-34BFC8F9F94D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2A1D41-77A6-4DB2-94A5-03C21B98E21E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17790" windowHeight="4500" xr2:uid="{32BA1DAC-DB74-DB41-A18F-C0D577D22603}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -889,6 +889,553 @@
   </si>
   <si>
     <t>text</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
+  </si>
+  <si>
+    <t>SB0001</t>
+  </si>
+  <si>
+    <t>As enacted, prohibits a healthcare provider from performing on a minor or administering to a minor a medical procedure if the performance or administration of the procedure is for the purpose of enabling a minor to identify with, or live as, a purported identity inconsistent with the minorâ€™s sex. - Amends TCA Title 28; Title 29; Title 33; Title 34; Title 36; Title 37; Title 39; Title 40; Title 49; Title 56; Title 63; Title 68 and Title 71.</t>
+  </si>
+  <si>
+    <t>https://legiscan.com/TN/bill/SB0001/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                           i                J
+                         Side ef J ettl!Msee
+                                  PUBLIC CHAPTER NO. 1
+                                         SENATE BILL NO. 1
+     By Johnson, Yager, Haile, Bowling, White, Crowe, Bailey, Hensley, Jackson, Reeves,
+                                   Stevens, Rose, Taylor
+                                   Substituted for: House Bill No. 1
+By Lamberth; Mr. Speaker Sexton; Faison, Garrett, Ragan, Zachary, Todd, Kumar, Rudder, Keisling,
+ Grills, White, Rudd, McCalmon, Sherrell, Capley, Warner, Richey, Raper, Littleton, Helton-Haynes,
+    Cochran, Fritts, Tim Hicks, Vital, Butler, Alexander, Haston, Darby, Moon, Crawford, Doggett,
+   Cepicky, Brock Martin, Hulsey, Slater, Hale, Hawk, Bricken, Williams, Bulso, Davis, Garringer,
+  Marsh, Howell, Lynn, Sparks, Gant, Leatherwood, Eldridge, Holsclaw, Reedy, Campbell, Baum,
+                                         Moody, Boyd, Powers
+AN ACT to amend Tennessee Code Annotated, Title 28; Title 29; Title 33; Title 34; Title 36; Title 37;
+     Title 39; Title 40; Title 49; Title 56; Title 63; Title 68 and Title 71, relative to medical care of
+     the young.
+BE IT ENACTED BY THE GENERAL ASSEMBLY OF THE STATE OF TENNESSEE:
+      SECTION 1. Tennessee Code Annotated, Title 68, is amended by adding the following as a
+new chapter:
+               68-33-101. Findings.
+                      (a) The legislature declares that it must take action to protect the health and
+               welfare of minors.
+                        (b) The legislature determines that medical procedures that alter a minor's
+               hormonal balance, remove a minor's sex organs, or otherwise change a minor's
+               physical appearance are harmful to a minor when these medical procedures are
+               performed for the purpose of enabling a minor to identify with, or live as, a purported
+               identity inconsistent with the minor's sex or treating purported discomfort or distress
+               from a discordance between the minor's sex and asserted identity. These procedures
+               can lead to the minor becoming irreversibly sterile, having increased risk of disease
+               and illness, or suffering from adverse and sometimes fatal psychological
+               consequences. Moreover, the legislature finds it likely that not all harmful effects
+               associated with these types of medical procedures when performed on a minor are
+               yet fully known, as many of these procedures, when performed on a minor for such
+               purposes, are experimental in nature and not supported by high-quality, long-term
+               medical studies.
+                       (c) The legislature determines that there is evidence that medical procedures
+               that alter a minor's hormonal balance, remove a minor's sex organs, or otherwise
+               change a minor's physical appearance are not consistent with professional medical
+               standards when the medical procedures are performed for the purpose of enabling a
+               minor to identify with, or live as, a purported identity inconsistent with the minor's sex
+               or treating purported discomfort or distress from a discordance between the minor's
+               sex and asserted identity because a minor's discordance can be resolved by less
+               invasive approaches that are likely to result in better outcomes for the minor.
+                      (d) The legislature finds that medical procedures are being performed on and
+               administered to minors in this state for such purposes, notwithstanding the risks and
+               harms to the minors.
+                      (e) The legislature finds that health authorities in Sweden, Finland, and the
+               United Kingdom have recognized similar trends and, after conducting systematic
+SB 1
+       reviews of the evidence, have found no evidence that the benefits of these
+       procedures outweigh the risks and thus have placed severe restrictions on their use.
+               (f) The legislature finds that Dr. John Money, one of the earliest advocates for
+       performing or administering such medical procedures on minors and a founder of the
+       Johns Hopkins Gender Identity Clinic, abused minors entrusted to his care, resulting
+       in the suicides of David and Brian Reimer.
+              (g) The legislature finds that such medical procedures are being performed on
+       and administered to minors in this state with rapidly increasing frequency and that
+       supposed guidelines advocating for such treatment have changed substantially in
+       recent years.
+               (h) The legislature finds that minors lack the maturity to fully understand and
+       appreciate the life-altering consequences of such procedures and that many
+       individuals have expressed regret for medical procedures that were performed on or
+       administered to them for such purposes when they were minors.
+               (i) The legislature finds that many of the same pharmaceutical companies that
+       contributed to the opioid epidemic have sought to profit from the administration of
+       drugs to or use of devices on minors for such purposes and have paid consulting fees
+       to physicians who then advocate for administration of drugs or use of devices for
+       such purposes.
+              0) The legislature finds that healthcare providers in this state have sought to
+       perform such surgeries on minors because of the financial incentive associated with
+       the surgeries, not necessarily because the surgeries are in a minor's best interest.
+              (k) The legislature finds that healthcare providers in this state have threatened
+       employees for conscientiously objecting, for religious, moral, or ethical reasons, to
+       performing or administering such medical procedures.
+               (I) The legislature finds that healthcare providers in this state have posted
+       pictures of naked minors online to advertise such surgeries.
+               (m) The legislature declares that the integrity and public respect of the medical
+       profession are significantly harmed by healthcare providers performing or
+       administering such medical procedures on minors. This state has a legitimate,
+       substantial, and compelling interest in protecting minors from physical and emotional
+       harm. This state has a legitimate, substantial, and compelling interest in protecting
+       the ability of minors to develop into adults who can create children of their own. This
+       state has a legitimate, substantial, and compelling interest in promoting the dignity of
+       minors. This state has a legitimate, substantial, and compelling interest in
+       encouraging minors to appreciate their sex, particularly as they undergo puberty. This
+       state has a legitimate, substantial, and compelling interest in protecting the integrity of
+       the medical profession, including by prohibiting medical procedures that are harmful,
+       unethical, immoral, experimental, or unsupported by high-quality or long-term studies,
+       or that might encourage minors to become disdainful of their sex.
+              (n) Therefore, it is the purpose of this chapter to prohibit medical procedures
+       from being administered to or performed on minors when the purpose of the medical
+       procedure is to:
+                     (1) Enable a minor to identify with, or live as, a purported identity
+              inconsistent with the minor's sex; or
+                     (2) Treat purported discomfort or distress from a discordance between
+              the minor's sex and asserted identity.
+       68-33-102. Definitions.
+       As used in this chapter:
+              (1) "Congenital defect" means a physical or chemical abnormality present in a
+       minor that is inconsistent with the normal development of a human being of the
+       minor's sex, including abnormalities caused by a medically verifiable disorder of sex
+       development, but does not include gender dysphoria, gender identity disorder, gender
+       incongruence, or any mental condition, disorder, disability, or abnormality;
+                                          2
+SB 1
+                 (2) "Healthcare provider" means a healthcare professional, establishment, or
+       facility licensed, registered, certified, or permitted pursuant to this title or title 63 and
+       under the regulatory authority of:.
+                       (A) The department of health;
+                      (8) An agency, board, council, or committee attached to the
+               department of health; or
+                       (C) The health facilities commission;
+               (3) "Hormone" means an androgen or estrogen;
+               (4) "Knowing" and "knowingly" have the same meaning as the term "knowing"
+       is defined in § 39-11-302;
+               (5) "Medical procedure" means:
+                       (A) Surgically removing, modifying, altering, or entering into tissues,
+               cavities, or organs of a human being; or
+                     (B) Prescribing, administering, or dispensing any puberty blocker or
+               hormone to a human being;
+               (6) "Minor" means an individual under eighteen (18) years of age;
+              (7) "Parent" means any biological, legal, or adoptive parent or parents of the
+       minor or any legal guardian of the minor;
+              (8) "Puberty blocker" means a drug or device that suppresses the production
+       of hormones in a minor's body to stop, delay, or suppress pubertal development; and
+              (9) "Sex" means a person's immutable characteristics of the reproductive
+       system that define the individual as male or female, as determined by anatomy and
+       genetics existing at the time of birth.
+       68-33-103. Prohibitions.
+               (a)(1) A healthcare provider shall not knowingly perform or offer to perform on
+               a minor, or administer or offer to administer to a minor, a medical procedure if
+               the performance or administration of the procedure is for the purpose of:
+                               (A) Enabling a minor to identify with, or live as, a purported
+                       identity inconsistent with the minor's sex; or
+                              (B) Treating purported discomfort or distress                from   a
+                       discordance between the minor's sex and asserted identity.
+                       (2) Subdivision (a)(1) applies to medical procedures that are:
+                               (A) Performed or administered in this state; or
+                               (B) Performed or administered on a minor located in this state,
+                       including via telehealth, as defined in§ 63-1-155.
+               (b )( 1) It is not a violation of subsection (a) if a healthcare provider knowingly
+               performs, or offers to perform, a medical procedure on or administers, or
+               offers to administer, a medical procedure to a minor if:                  ·
+                              (A) The performance or administration of the medical
+                       procedure is to treat a minor's congenital defect, precocious puberty,
+                       disease, or physical injury; or                        ·
+                              (B) The performance or administration of the medical
+                       procedure on the minor began prior to the effective date of this act and
+                       concludes on or before March 31, 2024.
+                      (2) For purposes of subdivision (b)(1 )(A), "disease" does not include
+               gender dysphoria, gender identity disorder, gender incongruence, or any
+               mental condition, disorder, disability, or abnormality.
+                                           3
+SB 1
+                             (3) For the exception in subdivision (b)(1 )(8) to apply, the minor's
+                     treating physician must certify in writing that, in the physician's good-faith
+                     medical judgment, based upon the facts known to the physician at the time,
+                     ending the medical procedure would be harmful to the minor. The certification
+                     must include the findings supporting the certification and must be made a part
+                     of the minor's medical record.
+                            (4) The exception in subdivision (b)(1)(8) does not allow a healthcare
+                     provider to perform or administer a medical procedure that is different from the
+                     medical procedure performed prior to the effective date of this act when the
+                     sole purpose of the subsequent medical procedure is to:
+                                     (A) Enable the minor to identify with, or live as, a purported
+                             identity inconsistent with the minor's sex; or
+                                   (8) Treat purported discomfort or distress from a discordance
+                             between the minor's sex and asserted identity.
+                     (c)(1) It is not a defense to any legal liability incurred as the result of a
+                     violation of this section that the minor, or a parent of the minor, consented to
+                     the conduct that constituted the violation.
+                              (2) This section supersedes any common law rule regarding a minor's
+                     ability to consent to a medical procedure that is performed or administered for
+                     the purpose of:
+                                     (A) Enabling the minor to identify with, or live as, a purported
+                             identity inconsistent with the minor's sex; or
+                                    (B) Treating purported discomfort or distress             from   a
+                             discordance between the minor's sex and asserted identity.
+              68-33-104. Distribution of Hormones or Puberty Blockers to Minors.
+              A person shall not knowingly provide a hormone or puberty blocker by any means to
+       a minor if the provision of the hormone or puberty blocker is not in compliance with this
+       chapter.
+              68-33-105. Private Right of Action.
+                     (a)(1) Except as otherwise provided in subdivision (a)(2), a minor, or the
+                     parent of a minor, injured as a result of a violation of this chapter, may bring a
+                     civil cause of action to recover compensatory damages, punitive damages,
+                     and reasonable attorney's fees, court costs, and expenses, against the
+                     healthcare provider alleged to have violated § 68-33-103 or any person
+                     alleged to have violated§ 68-33-104.
+                             (2) The parent of a minor injured as a result of a violation of this
+                     chapter shall not bring a civil cause of action against a healthcare provider or
+                     another person if the parent consented to the conduct that constituted the
+                     violation on behalf of the minor.
+                      (b) The parent or next of kin of a minor may bring a wrongful death action,
+              pursuant to title 20, chapter 5, part 1, against a healthcare provider alleged to have
+              violated § 68-33-103, if the injured minor is deceased and:
+                              (1) The minor's death is the result of the physical or emotional harm
+                     inflicted upon the minor by the violation; and
+                             (2) The parent of the minor did not consent to the conduct that
+                     constituted the violation on behalf of the minor.
+                       (c) If a court in any civil action brought pursuant to this section finds that a
+              healthcare provider knowingly violated § 68-33-103, then the court shall notify the
+              appropriate regulatory authority and the attorney general and reporter by mailing a
+              certified copy of the court's order to the regulatory authority and the attorney general
+              and reporter. Notification pursuant to this subsection (c) shall be made upon the
+              judgment of the court being made final.
+                     (d) For purposes of subsection (a), compensatory damages may include:
+                                                4
+S81
+                           (1) Reasonable economic losses caused by the emotional, mental, or
+                    physical effects of the violation, including, but not limited to:
+                                    (A) The cost of counseling, hospitalization, and any other
+                            medical expenses connected with treating the harm caused by the
+                            violation;
+                                   (8) Any out-of-pocket costs of the minor paid to the healthcare
+                            provider for the prohibited medical procedure; and
+                                    (C) Loss of income caused by the violation; and
+                             (2) Noneconomic damages caused by the violation, including, but not
+                    limited to, psychological and emotional anguish.
+                    (e) Notwithstanding any law to the contrary, an action commenced under this
+             section must be brought:
+                            (1) Within thirty (30) years from the date the minor reaches eighteen
+                     (18) years of age; or
+                            (2) Within ten (10) years of the minor's death if the minor dies.
+                      (f) This section ls declared to be remedial in nature, and this section must be
+             liberally construed to effectuate its purposes.
+             68-33-106. Attorney General and Reporter's Right of Action.
+                     (a) The attorney general and reporter shall establish a process by which
+             violations of this chapter may be reported.
+                     (b) The attorney general and reporter may bring an action against a
+             healthcare provider or any person that knowingly violates this chapter, within twenty
+             (20) years of the violation, to enjoin further violations, to disgorge any profits received
+             due to the medical procedure, and to recover a civil penalty of twenty-five thousand
+             dollars ($25,000) per violation. Each time a healthcare provider performs or
+             administers a medical procedure in violation of § 68-33-103 constitutes a separate
+             violation.
+                    (c) A civil penalty collected pursuant to this section must be paid into the
+             general fund of this state.
+                    (d) The attorney general and reporter is entitled to reasonable attorney's fees,
+             court costs, and expenses if the attorney general and reporter prevails in an action
+             brought pursuant to this section.
+                     (e) Jurisdiction for an action brought pursuant to this section is in the chancery
+             or circuit court of Williamson County or circuit court in the county where the violation
+             occurred.
+             68-33-107. Healthcare Provider Licensing Sanctions.
+              A violation of§ 68-33-103 constitutes a potential threat to public health, safety, and
+      welfare and requires emergency action by an alleged violator's appropriate regulatory
+      authority. Upon receiving notification pursuant to § 68-33-105(c), or upon otherwise
+      becoming aware of an alleged violation of § 68-33-103, the appropriate regulatory authority
+      shall proceed pursuant to title 63 or this title, as applicable.
+             68-33-108. Minor Immunity.
+              A minor upon whom a medical procedure is performed or administered must not be
+      held liable for violating this chapter.
+             68-33-109. Application.
+               This chapter does not prohibit or restrict psychological practice regulated pursuant to
+      title 63, chapter 11; the practice of professional counseling regulated pursuant to title 63,
+      chapter 22; or the practice of social work regulated pursuant to title 63, chapter 23.
+                                                5
+SB 1
+        SECTION 2. Tennessee Code Annotated, Section 63-1-169, is amended by deleting the
+section.
+        SECTION 3. If any provision of this act, or its application to any person or circumstance is
+held invalid, then the invalidity does not affect other provisions or applications of this act that can be
+given effect without the invalid provision or application, and to that end, the provisions of this act are
+severable.
+        SECTION 4. The headings in this act are for reference purposes only and do not constitute a
+part of the law enacted by this act. However, the Tennessee Code Commission is requested to
+include the headings in any compilation or publication containing this act.
+       SECTION 5. This act takes effect July 1, 2023, the public welfare requiring it, and applies to
+actions occurring on or after that date.
+                                                   6
+                       SENATE BILL NO.            1
+PASSED:          February 23, 2023
+                                                      RANDY McN
+                                             SPEAKER OF THE SE
+                                       C
+                                          CAMEfP"SEXTON,SPEAKER
+                                          HOUSE OF REPRESENTATIVES
+APPROVED this   {)..1,.o..    day of   fVlo,YcJ,        2023
+          ~l-                BILL LEE, GOVERNOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               68-33-101. Findings.
+                      (a) The legislature declares that it must take action to protect the health and
+               welfare of minors.
+                        (b) The legislature determines that medical procedures that alter a minor's
+               hormonal balance, remove a minor's sex organs, or otherwise change a minor's
+               physical appearance are harmful to a minor when these medical procedures are
+               performed for the purpose of enabling a minor to identify with, or live as, a purported
+               identity inconsistent with the minor's sex or treating purported discomfort or distress
+               from a discordance between the minor's sex and asserted identity. These procedures
+               can lead to the minor becoming irreversibly sterile, having increased risk of disease
+               and illness, or suffering from adverse and sometimes fatal psychological
+               consequences. Moreover, the legislature finds it likely that not all harmful effects
+               associated with these types of medical procedures when performed on a minor are
+               yet fully known, as many of these procedures, when performed on a minor for such
+               purposes, are experimental in nature and not supported by high-quality, long-term
+               medical studies.
+                       (c) The legislature determines that there is evidence that medical procedures
+               that alter a minor's hormonal balance, remove a minor's sex organs, or otherwise
+               change a minor's physical appearance are not consistent with professional medical
+               standards when the medical procedures are performed for the purpose of enabling a
+               minor to identify with, or live as, a purported identity inconsistent with the minor's sex
+               or treating purported discomfort or distress from a discordance between the minor's
+               sex and asserted identity because a minor's discordance can be resolved by less
+               invasive approaches that are likely to result in better outcomes for the minor.
+                      (d) The legislature finds that medical procedures are being performed on and
+               administered to minors in this state for such purposes, notwithstanding the risks and
+               harms to the minors.
+                      (e) The legislature finds that health authorities in Sweden, Finland, and the
+               United Kingdom have recognized similar trends and, after conducting systematic
+SB 1
+       reviews of the evidence, have found no evidence that the benefits of these
+       procedures outweigh the risks and thus have placed severe restrictions on their use.
+               (f) The legislature finds that Dr. John Money, one of the earliest advocates for
+       performing or administering such medical procedures on minors and a founder of the
+       Johns Hopkins Gender Identity Clinic, abused minors entrusted to his care, resulting
+       in the suicides of David and Brian Reimer.
+              (g) The legislature finds that such medical procedures are being performed on
+       and administered to minors in this state with rapidly increasing frequency and that
+       supposed guidelines advocating for such treatment have changed substantially in
+       recent years.
+               (h) The legislature finds that minors lack the maturity to fully understand and
+       appreciate the life-altering consequences of such procedures and that many
+       individuals have expressed regret for medical procedures that were performed on or
+       administered to them for such purposes when they were minors.
+               (i) The legislature finds that many of the same pharmaceutical companies that
+       contributed to the opioid epidemic have sought to profit from the administration of
+       drugs to or use of devices on minors for such purposes and have paid consulting fees
+       to physicians who then advocate for administration of drugs or use of devices for
+       such purposes.
+              0) The legislature finds that healthcare providers in this state have sought to
+       perform such surgeries on minors because of the financial incentive associated with
+       the surgeries, not necessarily because the surgeries are in a minor's best interest.
+              (k) The legislature finds that healthcare providers in this state have threatened
+       employees for conscientiously objecting, for religious, moral, or ethical reasons, to
+       performing or administering such medical procedures.
+               (I) The legislature finds that healthcare providers in this state have posted
+       pictures of naked minors online to advertise such surgeries.
+               (m) The legislature declares that the integrity and public respect of the medical
+       profession are significantly harmed by healthcare providers performing or
+       administering such medical procedures on minors. This state has a legitimate,
+       substantial, and compelling interest in protecting minors from physical and emotional
+       harm. This state has a legitimate, substantial, and compelling interest in protecting
+       the ability of minors to develop into adults who can create children of their own. This
+       state has a legitimate, substantial, and compelling interest in promoting the dignity of
+       minors. This state has a legitimate, substantial, and compelling interest in
+       encouraging minors to appreciate their sex, particularly as they undergo puberty. This
+       state has a legitimate, substantial, and compelling interest in protecting the integrity of
+       the medical profession, including by prohibiting medical procedures that are harmful,
+       unethical, immoral, experimental, or unsupported by high-quality or long-term studies,
+       or that might encourage minors to become disdainful of their sex.
+              (n) Therefore, it is the purpose of this chapter to prohibit medical procedures
+       from being administered to or performed on minors when the purpose of the medical
+       procedure is to:
+                     (1) Enable a minor to identify with, or live as, a purported identity
+              inconsistent with the minor's sex; or
+                     (2) Treat purported discomfort or distress from a discordance between
+              the minor's sex and asserted identity.
+       68-33-102. Definitions.
+       As used in this chapter:
+              (1) "Congenital defect" means a physical or chemical abnormality present in a
+       minor that is inconsistent with the normal development of a human being of the
+       minor's sex, including abnormalities caused by a medically verifiable disorder of sex
+       development, but does not include gender dysphoria, gender identity disorder, gender
+       incongruence, or any mental condition, disorder, disability, or abnormality;
+                                          2
+SB 1
+                 (2) "Healthcare provider" means a healthcare professional, establishment, or
+       facility licensed, registered, certified, or permitted pursuant to this title or title 63 and
+       under the regulatory authority of:.
+                       (A) The department of health;
+                      (8) An agency, board, council, or committee attached to the
+               department of health; or
+                       (C) The health facilities commission;
+               (3) "Hormone" means an androgen or estrogen;
+               (4) "Knowing" and "knowingly" have the same meaning as the term "knowing"
+       is defined in § 39-11-302;
+               (5) "Medical procedure" means:
+                       (A) Surgically removing, modifying, altering, or entering into tissues,
+               cavities, or organs of a human being; or
+                     (B) Prescribing, administering, or dispensing any puberty blocker or
+               hormone to a human being;
+               (6) "Minor" means an individual under eighteen (18) years of age;
+              (7) "Parent" means any biological, legal, or adoptive parent or parents of the
+       minor or any legal guardian of the minor;
+              (8) "Puberty blocker" means a drug or device that suppresses the production
+       of hormones in a minor's body to stop, delay, or suppress pubertal development; and
+              (9) "Sex" means a person's immutable characteristics of the reproductive
+       system that define the individual as male or female, as determined by anatomy and
+       genetics existing at the time of birth.
+       68-33-103. Prohibitions.
+               (a)(1) A healthcare provider shall not knowingly perform or offer to perform on
+               a minor, or administer or offer to administer to a minor, a medical procedure if
+               the performance or administration of the procedure is for the purpose of:
+                               (A) Enabling a minor to identify with, or live as, a purported
+                       identity inconsistent with the minor's sex; or
+                              (B) Treating purported discomfort or distress                from   a
+                       discordance between the minor's sex and asserted identity.
+                       (2) Subdivision (a)(1) applies to medical procedures that are:
+                               (A) Performed or administered in this state; or
+                               (B) Performed or administered on a minor located in this state,
+                       including via telehealth, as defined in§ 63-1-155.
+               (b )( 1) It is not a violation of subsection (a) if a healthcare provider knowingly
+               performs, or offers to perform, a medical procedure on or administers, or
+               offers to administer, a medical procedure to a minor if:                  ·
+                              (A) The performance or administration of the medical
+                       procedure is to treat a minor's congenital defect, precocious puberty,
+                       disease, or physical injury; or                        ·
+                              (B) The performance or administration of the medical
+                       procedure on the minor began prior to the effective date of this act and
+                       concludes on or before March 31, 2024.
+                      (2) For purposes of subdivision (b)(1 )(A), "disease" does not include
+               gender dysphoria, gender identity disorder, gender incongruence, or any
+               mental condition, disorder, disability, or abnormality.
+                                           3
+SB 1
+                             (3) For the exception in subdivision (b)(1 )(8) to apply, the minor's
+                     treating physician must certify in writing that, in the physician's good-faith
+                     medical judgment, based upon the facts known to the physician at the time,
+                     ending the medical procedure would be harmful to the minor. The certification
+                     must include the findings supporting the certification and must be made a part
+                     of the minor's medical record.
+                            (4) The exception in subdivision (b)(1)(8) does not allow a healthcare
+                     provider to perform or administer a medical procedure that is different from the
+                     medical procedure performed prior to the effective date of this act when the
+                     sole purpose of the subsequent medical procedure is to:
+                                     (A) Enable the minor to identify with, or live as, a purported
+                             identity inconsistent with the minor's sex; or
+                                   (8) Treat purported discomfort or distress from a discordance
+                             between the minor's sex and asserted identity.
+                     (c)(1) It is not a defense to any legal liability incurred as the result of a
+                     violation of this section that the minor, or a parent of the minor, consented to
+                     the conduct that constituted the violation.
+                              (2) This section supersedes any common law rule regarding a minor's
+                     ability to consent to a medical procedure that is performed or administered for
+                     the purpose of:
+                                     (A) Enabling the minor to identify with, or live as, a purported
+                             identity inconsistent with the minor's sex; or
+                                    (B) Treating purported discomfort or distress             from   a
+                             discordance between the minor's sex and asserted identity.
+              68-33-104. Distribution of Hormones or Puberty Blockers to Minors.
+              A person shall not knowingly provide a hormone or puberty blocker by any means to
+       a minor if the provision of the hormone or puberty blocker is not in compliance with this
+       chapter.
+              68-33-105. Private Right of Action.
+                     (a)(1) Except as otherwise provided in subdivision (a)(2), a minor, or the
+                     parent of a minor, injured as a result of a violation of this chapter, may bring a
+                     civil cause of action to recover compensatory damages, punitive damages,
+                     and reasonable attorney's fees, court costs, and expenses, against the
+                     healthcare provider alleged to have violated § 68-33-103 or any person
+                     alleged to have violated§ 68-33-104.
+                             (2) The parent of a minor injured as a result of a violation of this
+                     chapter shall not bring a civil cause of action against a healthcare provider or
+                     another person if the parent consented to the conduct that constituted the
+                     violation on behalf of the minor.
+                      (b) The parent or next of kin of a minor may bring a wrongful death action,
+              pursuant to title 20, chapter 5, part 1, against a healthcare provider alleged to have
+              violated § 68-33-103, if the injured minor is deceased and:
+                              (1) The minor's death is the result of the physical or emotional harm
+                     inflicted upon the minor by the violation; and
+                             (2) The parent of the minor did not consent to the conduct that
+                     constituted the violation on behalf of the minor.
+                       (c) If a court in any civil action brought pursuant to this section finds that a
+              healthcare provider knowingly violated § 68-33-103, then the court shall notify the
+              appropriate regulatory authority and the attorney general and reporter by mailing a
+              certified copy of the court's order to the regulatory authority and the attorney general
+              and reporter. Notification pursuant to this subsection (c) shall be made upon the
+              judgment of the court being made final.
+                     (d) For purposes of subsection (a), compensatory damages may include:
+                                                4
+S81
+                           (1) Reasonable economic losses caused by the emotional, mental, or
+                    physical effects of the violation, including, but not limited to:
+                                    (A) The cost of counseling, hospitalization, and any other
+                            medical expenses connected with treating the harm caused by the
+                            violation;
+                                   (8) Any out-of-pocket costs of the minor paid to the healthcare
+                            provider for the prohibited medical procedure; and
+                                    (C) Loss of income caused by the violation; and
+                             (2) Noneconomic damages caused by the violation, including, but not
+                    limited to, psychological and emotional anguish.
+                    (e) Notwithstanding any law to the contrary, an action commenced under this
+             section must be brought:
+                            (1) Within thirty (30) years from the date the minor reaches eighteen
+                     (18) years of age; or
+                            (2) Within ten (10) years of the minor's death if the minor dies.
+                      (f) This section ls declared to be remedial in nature, and this section must be
+             liberally construed to effectuate its purposes.
+             68-33-106. Attorney General and Reporter's Right of Action.
+                     (a) The attorney general and reporter shall establish a process by which
+             violations of this chapter may be reported.
+                     (b) The attorney general and reporter may bring an action against a
+             healthcare provider or any person that knowingly violates this chapter, within twenty
+             (20) years of the violation, to enjoin further violations, to disgorge any profits received
+             due to the medical procedure, and to recover a civil penalty of twenty-five thousand
+             dollars ($25,000) per violation. Each time a healthcare provider performs or
+             administers a medical procedure in violation of § 68-33-103 constitutes a separate
+             violation.
+                    (c) A civil penalty collected pursuant to this section must be paid into the
+             general fund of this state.
+                    (d) The attorney general and reporter is entitled to reasonable attorney's fees,
+             court costs, and expenses if the attorney general and reporter prevails in an action
+             brought pursuant to this section.
+                     (e) Jurisdiction for an action brought pursuant to this section is in the chancery
+             or circuit court of Williamson County or circuit court in the county where the violation
+             occurred.
+             68-33-107. Healthcare Provider Licensing Sanctions.
+              A violation of§ 68-33-103 constitutes a potential threat to public health, safety, and
+      welfare and requires emergency action by an alleged violator's appropriate regulatory
+      authority. Upon receiving notification pursuant to § 68-33-105(c), or upon otherwise
+      becoming aware of an alleged violation of § 68-33-103, the appropriate regulatory authority
+      shall proceed pursuant to title 63 or this title, as applicable.
+             68-33-108. Minor Immunity.
+              A minor upon whom a medical procedure is performed or administered must not be
+      held liable for violating this chapter.
+             68-33-109. Application.
+               This chapter does not prohibit or restrict psychological practice regulated pursuant to
+      title 63, chapter 11; the practice of professional counseling regulated pursuant to title 63,
+      chapter 22; or the practice of social work regulated pursuant to title 63, chapter 23.
+                                                5
+SB 1
+        SECTION 2. Tennessee Code Annotated, Section 63-1-169, is amended by deleting the
+section.
+        SECTION 3. If any provision of this act, or its application to any person or circumstance is
+held invalid, then the invalidity does not affect other provisions or applications of this act that can be
+given effect without the invalid provision or application, and to that end, the provisions of this act are
+severable.
+        SECTION 4. The headings in this act are for reference purposes only and do not constitute a
+part of the law enacted by this act. However, the Tennessee Code Commission is requested to
+include the headings in any compilation or publication containing this act.
+       SECTION 5. This act takes effect July 1, 2023, the public welfare requiring it, and applies to
+actions occurring on or after that date.</t>
   </si>
 </sst>
 </file>
@@ -1257,15 +1804,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{968883DB-AF00-B64D-9E18-9ACE2911B86F}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="29.83203125" customWidth="1"/>
     <col min="7" max="7" width="31.5" customWidth="1"/>
-    <col min="8" max="8" width="69.5" customWidth="1"/>
+    <col min="8" max="8" width="57.58203125" customWidth="1"/>
     <col min="9" max="9" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1414,8 +1961,34 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
+    <row r="6" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>45007</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
@@ -1426,6 +1999,7 @@
     <hyperlink ref="G3" r:id="rId2" xr:uid="{9C3C9FB3-D6AF-B94B-8F48-0A596008A7B2}"/>
     <hyperlink ref="G4" r:id="rId3" xr:uid="{B0CA5216-FFC3-4B48-9BB3-EA444DB03F7F}"/>
     <hyperlink ref="G5" r:id="rId4" xr:uid="{D2457618-5E35-E147-A877-40D977BB6266}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{999F8CF2-C2A8-4381-A51D-6662DD111500}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>